<commit_message>
added relevance to output message
</commit_message>
<xml_diff>
--- a/.Lists_for_T.xlsx
+++ b/.Lists_for_T.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\PycharmProjects\pythonProject_TranslatorMeets Zen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E25E991-0D8B-4B61-9E57-353348A794E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2E890F-3C49-48F5-A762-CECC16F63C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A4ABEF32-ABB1-47D8-A5EA-945E0E66EE28}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>идентификаторы</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>актуальность</t>
+  </si>
+  <si>
+    <t>нет данных</t>
+  </si>
+  <si>
+    <t>нет данных!</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,6 +618,9 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
@@ -623,6 +632,9 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
@@ -634,6 +646,9 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
@@ -645,6 +660,9 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
@@ -656,6 +674,9 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
@@ -667,6 +688,9 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
@@ -675,6 +699,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
@@ -683,6 +710,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
@@ -691,6 +721,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
@@ -709,7 +742,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,6 +778,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
@@ -756,6 +792,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
@@ -767,6 +806,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>36</v>
       </c>
@@ -778,6 +820,9 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
@@ -789,6 +834,9 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>40</v>
       </c>
@@ -800,6 +848,9 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
@@ -808,6 +859,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
@@ -816,6 +870,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
cleaned up a bit, added a message (no relevance data, need access)
</commit_message>
<xml_diff>
--- a/.Lists_for_T.xlsx
+++ b/.Lists_for_T.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\PycharmProjects\pythonProject_TranslatorMeets Zen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2E890F-3C49-48F5-A762-CECC16F63C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7F2A81-DE6D-4577-9E96-F98CB083C8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A4ABEF32-ABB1-47D8-A5EA-945E0E66EE28}"/>
+    <workbookView minimized="1" xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{A4ABEF32-ABB1-47D8-A5EA-945E0E66EE28}"/>
   </bookViews>
   <sheets>
     <sheet name="управление" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>идентификаторы</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>нет данных</t>
-  </si>
-  <si>
-    <t>нет данных!</t>
   </si>
 </sst>
 </file>
@@ -581,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E246C7-557F-43C9-A2FF-F041F12063BE}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,7 +686,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
@@ -741,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE878CED-5586-44F7-9198-BCEF99FB6A4B}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>